<commit_message>
chore: Update API endpoint paths and add SaveIndividual function
</commit_message>
<xml_diff>
--- a/docs/TMF632 Detail mapping.xlsx
+++ b/docs/TMF632 Detail mapping.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://truecorp-my.sharepoint.com/personal/chailuck_truecorp_co_th/Documents/DTAC/Project/2024-023 VC-CRM - NOM/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Pop\Knowledge\Programming\GO lang\tmfEcho\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="551" documentId="8_{1D22A2F4-9947-4A33-93EA-AD0AEFC50B13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7E9C7C6C-7B25-4F7A-AD30-56AB85B7FDCB}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2CDD576-4B15-4CA3-98AB-DB7E73BC0DAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{E394FAEC-399A-4A89-9DDB-9CA6A4425705}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="32640" windowHeight="21120" xr2:uid="{E394FAEC-399A-4A89-9DDB-9CA6A4425705}"/>
   </bookViews>
   <sheets>
     <sheet name="TMF632 - Individual" sheetId="1" r:id="rId1"/>
@@ -29,8 +29,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -2114,10 +2112,10 @@
   <dimension ref="A1:U220"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="G24" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="O23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G32" sqref="G32"/>
+      <selection pane="bottomRight" activeCell="R33" sqref="R33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2986,7 +2984,7 @@
         <v>5</v>
       </c>
       <c r="G21" s="8" t="str">
-        <f t="shared" si="1"/>
+        <f>UPPER(LEFT(E21,1))&amp;RIGHT(E21,LEN(E21)-1)&amp;" "&amp;F21&amp;" `json:"""&amp;A21&amp;""""&amp;"`"</f>
         <v>Title string `json:"title"`</v>
       </c>
       <c r="H21" s="24"/>
@@ -10335,6 +10333,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Detail mapping for TMF632 changed
</commit_message>
<xml_diff>
--- a/docs/TMF632 Detail mapping.xlsx
+++ b/docs/TMF632 Detail mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Pop\Knowledge\Programming\GO lang\tmfEcho\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2CDD576-4B15-4CA3-98AB-DB7E73BC0DAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8BBBE81-76DC-4DF8-BDFD-C635457720AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="32640" windowHeight="21120" xr2:uid="{E394FAEC-399A-4A89-9DDB-9CA6A4425705}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="32640" windowHeight="21120" activeTab="2" xr2:uid="{E394FAEC-399A-4A89-9DDB-9CA6A4425705}"/>
   </bookViews>
   <sheets>
     <sheet name="TMF632 - Individual" sheetId="1" r:id="rId1"/>
@@ -2111,11 +2111,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{176DAE2C-8628-4777-B02F-B10D1CA19D22}">
   <dimension ref="A1:U220"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="O23" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane xSplit="6" ySplit="1" topLeftCell="O29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R33" sqref="R33"/>
+      <selection pane="bottomRight" activeCell="R35" sqref="R35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3127,7 +3127,7 @@
       <c r="S24" s="12"/>
       <c r="T24" s="12"/>
     </row>
-    <row r="25" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" ht="130.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
       <c r="B25" s="13" t="s">
         <v>41</v>
@@ -3247,7 +3247,7 @@
       <c r="S27" s="15"/>
       <c r="T27" s="15"/>
     </row>
-    <row r="28" spans="1:20" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
       <c r="B28" s="13" t="s">
         <v>40</v>
@@ -3327,7 +3327,7 @@
       <c r="S29" s="14"/>
       <c r="T29" s="14"/>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
       <c r="B30" s="13" t="s">
         <v>46</v>
@@ -10918,8 +10918,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5A045D9-C774-43CC-A709-A07349342DD9}">
   <dimension ref="A1:A271"/>
   <sheetViews>
-    <sheetView topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="N107" sqref="N107"/>
+    <sheetView tabSelected="1" topLeftCell="A193" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J205" sqref="J205"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>